<commit_message>
Ajout WatchDog 60 min ; release date en parametre ; é ° suppressed
</commit_message>
<xml_diff>
--- a/Wifi-thermo-num/Cablage_themo_thingspeaks.xlsx
+++ b/Wifi-thermo-num/Cablage_themo_thingspeaks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="17220" windowHeight="5385" tabRatio="691" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="17220" windowHeight="5385" tabRatio="691" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HW ref" sheetId="11" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="FDTI" sheetId="7" r:id="rId6"/>
     <sheet name="Power supply" sheetId="10" r:id="rId7"/>
     <sheet name="thermo num" sheetId="14" r:id="rId8"/>
+    <sheet name="Interface" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="216">
   <si>
     <t>Int</t>
   </si>
@@ -675,6 +676,102 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>For Debug / flashing / with power supplu needed:</t>
+  </si>
+  <si>
+    <t>PC side</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>FDTI</t>
+  </si>
+  <si>
+    <t>5V/3V</t>
+  </si>
+  <si>
+    <t>DB9 M</t>
+  </si>
+  <si>
+    <t>USB to DB9</t>
+  </si>
+  <si>
+    <t>Arduino side</t>
+  </si>
+  <si>
+    <t>DB9 F</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>VCC (5v/3v)</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Slave</t>
+  </si>
+  <si>
+    <t>VCC5v</t>
+  </si>
+  <si>
+    <t>Data-</t>
+  </si>
+  <si>
+    <t>Data+</t>
+  </si>
+  <si>
+    <t>For Debug / flashing / NO power supply needed:</t>
+  </si>
+  <si>
+    <t>Interface for sensors</t>
+  </si>
+  <si>
+    <t>Sensor side</t>
+  </si>
+  <si>
+    <t>ONE wire</t>
+  </si>
+  <si>
+    <t>Vcc</t>
+  </si>
+  <si>
+    <t>OneWire</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>Sensor1</t>
+  </si>
+  <si>
+    <t>Sensor2</t>
+  </si>
+  <si>
+    <t>Sensor3</t>
+  </si>
+  <si>
+    <t>Sensor4</t>
+  </si>
+  <si>
+    <t>Sensor plug</t>
+  </si>
+  <si>
+    <t>Slave Prog plug</t>
+  </si>
+  <si>
+    <t>RST</t>
   </si>
 </sst>
 </file>
@@ -917,7 +1014,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1395,6 +1492,50 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1406,7 +1547,7 @@
     </xf>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1690,6 +1831,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -5650,8 +5815,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6966858" y="22029963"/>
-          <a:ext cx="3918856" cy="2397085"/>
+          <a:off x="6975663" y="23599587"/>
+          <a:ext cx="3919416" cy="2349862"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5690,8 +5855,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7075713" y="24601715"/>
-          <a:ext cx="2258786" cy="2181782"/>
+          <a:off x="7084518" y="26598763"/>
+          <a:ext cx="2259346" cy="2134557"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6704,7 +6869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -6981,26 +7146,26 @@
         <v>10</v>
       </c>
       <c r="B12" s="56"/>
-      <c r="P12" s="148" t="s">
+      <c r="P12" s="149" t="s">
         <v>178</v>
       </c>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="148"/>
-      <c r="T12" s="148"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="148"/>
-      <c r="W12" s="148"/>
-      <c r="AD12" s="148" t="s">
+      <c r="Q12" s="149"/>
+      <c r="R12" s="149"/>
+      <c r="S12" s="149"/>
+      <c r="T12" s="149"/>
+      <c r="U12" s="149"/>
+      <c r="V12" s="149"/>
+      <c r="W12" s="149"/>
+      <c r="AD12" s="149" t="s">
         <v>177</v>
       </c>
-      <c r="AE12" s="148"/>
-      <c r="AF12" s="148"/>
-      <c r="AG12" s="148"/>
-      <c r="AH12" s="148"/>
-      <c r="AI12" s="148"/>
-      <c r="AJ12" s="148"/>
-      <c r="AK12" s="148"/>
+      <c r="AE12" s="149"/>
+      <c r="AF12" s="149"/>
+      <c r="AG12" s="149"/>
+      <c r="AH12" s="149"/>
+      <c r="AI12" s="149"/>
+      <c r="AJ12" s="149"/>
+      <c r="AK12" s="149"/>
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="19" t="s">
@@ -7461,22 +7626,22 @@
       <c r="H35" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="Y35" s="148" t="s">
+      <c r="Y35" s="149" t="s">
         <v>176</v>
       </c>
-      <c r="Z35" s="148"/>
-      <c r="AA35" s="148"/>
-      <c r="AB35" s="148"/>
-      <c r="AC35" s="148"/>
-      <c r="AD35" s="148"/>
-      <c r="AE35" s="148"/>
-      <c r="AF35" s="148"/>
-      <c r="AG35" s="148"/>
-      <c r="AH35" s="148"/>
-      <c r="AI35" s="148"/>
-      <c r="AJ35" s="148"/>
-      <c r="AK35" s="148"/>
-      <c r="AL35" s="148"/>
+      <c r="Z35" s="149"/>
+      <c r="AA35" s="149"/>
+      <c r="AB35" s="149"/>
+      <c r="AC35" s="149"/>
+      <c r="AD35" s="149"/>
+      <c r="AE35" s="149"/>
+      <c r="AF35" s="149"/>
+      <c r="AG35" s="149"/>
+      <c r="AH35" s="149"/>
+      <c r="AI35" s="149"/>
+      <c r="AJ35" s="149"/>
+      <c r="AK35" s="149"/>
+      <c r="AL35" s="149"/>
     </row>
     <row r="36" spans="1:38">
       <c r="A36" s="63"/>
@@ -7727,8 +7892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8479,7 +8644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -8507,4 +8672,872 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="6" width="11.42578125" style="148"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="150" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="145"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="150" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150" t="s">
+        <v>198</v>
+      </c>
+      <c r="J2" s="150"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="150" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="150"/>
+      <c r="C3" s="150" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="150"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="152" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="153"/>
+      <c r="C4" s="151" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="J4" s="151" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="151">
+        <v>1</v>
+      </c>
+      <c r="B5" s="151" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="151">
+        <v>1</v>
+      </c>
+      <c r="D5" s="151" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="151"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151">
+        <v>1</v>
+      </c>
+      <c r="H5" s="151" t="s">
+        <v>194</v>
+      </c>
+      <c r="I5" s="151" t="s">
+        <v>194</v>
+      </c>
+      <c r="J5" s="151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="151">
+        <v>2</v>
+      </c>
+      <c r="B6" s="151" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="151">
+        <v>2</v>
+      </c>
+      <c r="D6" s="151" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151">
+        <v>2</v>
+      </c>
+      <c r="H6" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="I6" s="151" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" s="151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="151">
+        <v>3</v>
+      </c>
+      <c r="B7" s="151" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="151">
+        <v>3</v>
+      </c>
+      <c r="D7" s="151" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151">
+        <v>3</v>
+      </c>
+      <c r="H7" s="151" t="s">
+        <v>195</v>
+      </c>
+      <c r="I7" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="J7" s="151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="151">
+        <v>4</v>
+      </c>
+      <c r="B8" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="151">
+        <v>4</v>
+      </c>
+      <c r="D8" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="151"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="151">
+        <v>4</v>
+      </c>
+      <c r="H8" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="151">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="145"/>
+      <c r="B9" s="145"/>
+      <c r="C9" s="145"/>
+      <c r="D9" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="151"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="151">
+        <v>5</v>
+      </c>
+      <c r="H9" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="151">
+        <v>6</v>
+      </c>
+      <c r="H10" s="151"/>
+      <c r="I10" s="151"/>
+      <c r="J10" s="151">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151">
+        <v>7</v>
+      </c>
+      <c r="H11" s="151"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="D12" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151">
+        <v>8</v>
+      </c>
+      <c r="H12" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="151">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="D13" s="151"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="151"/>
+      <c r="G13" s="151">
+        <v>9</v>
+      </c>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="151">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="150" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="150"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
+      <c r="H15" s="150"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="150"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="145"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="150" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="150"/>
+      <c r="E16" s="150"/>
+      <c r="F16" s="150"/>
+      <c r="G16" s="150"/>
+      <c r="H16" s="150"/>
+      <c r="I16" s="150" t="s">
+        <v>214</v>
+      </c>
+      <c r="J16" s="150"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="150" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="150"/>
+      <c r="C17" s="150" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="150"/>
+      <c r="E17" s="150"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="150"/>
+      <c r="H17" s="150"/>
+      <c r="I17" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="J17" s="150"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="152" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="153"/>
+      <c r="C18" s="151" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151" t="s">
+        <v>189</v>
+      </c>
+      <c r="H18" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="I18" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="J18" s="151" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="151">
+        <v>1</v>
+      </c>
+      <c r="B19" s="151" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="151">
+        <v>1</v>
+      </c>
+      <c r="D19" s="151" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151">
+        <v>1</v>
+      </c>
+      <c r="H19" s="151" t="s">
+        <v>194</v>
+      </c>
+      <c r="I19" s="151" t="s">
+        <v>194</v>
+      </c>
+      <c r="J19" s="151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="151">
+        <v>2</v>
+      </c>
+      <c r="B20" s="151" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="151">
+        <v>2</v>
+      </c>
+      <c r="D20" s="151" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151">
+        <v>2</v>
+      </c>
+      <c r="H20" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="I20" s="151" t="s">
+        <v>195</v>
+      </c>
+      <c r="J20" s="151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="151">
+        <v>3</v>
+      </c>
+      <c r="B21" s="151" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="151">
+        <v>3</v>
+      </c>
+      <c r="D21" s="151" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
+      <c r="G21" s="151">
+        <v>3</v>
+      </c>
+      <c r="H21" s="151" t="s">
+        <v>195</v>
+      </c>
+      <c r="I21" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="J21" s="151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="151">
+        <v>4</v>
+      </c>
+      <c r="B22" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="151">
+        <v>4</v>
+      </c>
+      <c r="D22" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="151"/>
+      <c r="F22" s="151"/>
+      <c r="G22" s="151">
+        <v>4</v>
+      </c>
+      <c r="H22" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="151">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="145"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="145"/>
+      <c r="D23" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="151"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151">
+        <v>5</v>
+      </c>
+      <c r="H23" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="D24" s="151"/>
+      <c r="E24" s="151"/>
+      <c r="F24" s="151"/>
+      <c r="G24" s="151">
+        <v>6</v>
+      </c>
+      <c r="H24" s="151"/>
+      <c r="I24" s="151"/>
+      <c r="J24" s="151">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="D25" s="151"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
+      <c r="G25" s="151">
+        <v>7</v>
+      </c>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="D26" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="151"/>
+      <c r="F26" s="151"/>
+      <c r="G26" s="151">
+        <v>8</v>
+      </c>
+      <c r="H26" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="151">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="D27" s="151"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151">
+        <v>9</v>
+      </c>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="151">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="150" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="150"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="150"/>
+      <c r="C30" s="150" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="150"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="156"/>
+      <c r="I30" s="156"/>
+      <c r="J30" s="157"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="150" t="s">
+        <v>213</v>
+      </c>
+      <c r="B31" s="150"/>
+      <c r="C31" s="150" t="s">
+        <v>205</v>
+      </c>
+      <c r="D31" s="150"/>
+      <c r="E31" s="154" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" s="155"/>
+      <c r="G31" s="151" t="s">
+        <v>209</v>
+      </c>
+      <c r="H31" s="151" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="151" t="s">
+        <v>211</v>
+      </c>
+      <c r="J31" s="151" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="151" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" s="151" t="s">
+        <v>192</v>
+      </c>
+      <c r="D32" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="E32" s="151" t="s">
+        <v>192</v>
+      </c>
+      <c r="F32" s="151" t="s">
+        <v>193</v>
+      </c>
+      <c r="G32" s="151" t="s">
+        <v>192</v>
+      </c>
+      <c r="H32" s="151" t="s">
+        <v>192</v>
+      </c>
+      <c r="I32" s="151" t="s">
+        <v>192</v>
+      </c>
+      <c r="J32" s="151" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="151" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" s="151">
+        <v>1</v>
+      </c>
+      <c r="C33" s="151">
+        <v>1</v>
+      </c>
+      <c r="D33" s="151" t="s">
+        <v>206</v>
+      </c>
+      <c r="E33" s="151" t="s">
+        <v>206</v>
+      </c>
+      <c r="F33" s="151">
+        <v>1</v>
+      </c>
+      <c r="G33" s="151" t="s">
+        <v>206</v>
+      </c>
+      <c r="H33" s="151" t="s">
+        <v>206</v>
+      </c>
+      <c r="I33" s="151" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" s="151" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="151" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="151">
+        <v>2</v>
+      </c>
+      <c r="C34" s="151"/>
+      <c r="D34" s="151"/>
+      <c r="E34" s="151" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="151">
+        <v>2</v>
+      </c>
+      <c r="G34" s="151"/>
+      <c r="H34" s="151"/>
+      <c r="I34" s="151"/>
+      <c r="J34" s="151"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="151">
+        <v>3</v>
+      </c>
+      <c r="C35" s="151"/>
+      <c r="D35" s="151"/>
+      <c r="E35" s="151" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="151">
+        <v>3</v>
+      </c>
+      <c r="G35" s="151"/>
+      <c r="H35" s="151"/>
+      <c r="I35" s="151"/>
+      <c r="J35" s="151"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="151" t="s">
+        <v>209</v>
+      </c>
+      <c r="B36" s="151">
+        <v>4</v>
+      </c>
+      <c r="C36" s="151"/>
+      <c r="D36" s="151"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="151"/>
+      <c r="G36" s="151" t="s">
+        <v>209</v>
+      </c>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="151"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="151">
+        <v>5</v>
+      </c>
+      <c r="C37" s="151">
+        <v>5</v>
+      </c>
+      <c r="D37" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="151">
+        <v>5</v>
+      </c>
+      <c r="G37" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" s="151" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="158" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" s="151">
+        <v>6</v>
+      </c>
+      <c r="C38" s="151">
+        <v>6</v>
+      </c>
+      <c r="D38" s="151" t="s">
+        <v>205</v>
+      </c>
+      <c r="E38" s="151"/>
+      <c r="F38" s="151">
+        <v>6</v>
+      </c>
+      <c r="G38" s="151"/>
+      <c r="H38" s="151"/>
+      <c r="I38" s="151"/>
+      <c r="J38" s="151"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="151" t="s">
+        <v>210</v>
+      </c>
+      <c r="B39" s="151">
+        <v>7</v>
+      </c>
+      <c r="C39" s="151"/>
+      <c r="D39" s="151"/>
+      <c r="E39" s="151"/>
+      <c r="F39" s="151"/>
+      <c r="G39" s="151"/>
+      <c r="H39" s="151" t="s">
+        <v>210</v>
+      </c>
+      <c r="I39" s="151"/>
+      <c r="J39" s="151"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="151" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="151">
+        <v>8</v>
+      </c>
+      <c r="C40" s="151"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="151"/>
+      <c r="F40" s="151"/>
+      <c r="G40" s="151"/>
+      <c r="H40" s="151"/>
+      <c r="I40" s="151" t="s">
+        <v>211</v>
+      </c>
+      <c r="J40" s="151"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="151" t="s">
+        <v>212</v>
+      </c>
+      <c r="B41" s="151">
+        <v>9</v>
+      </c>
+      <c r="C41" s="151"/>
+      <c r="D41" s="151"/>
+      <c r="E41" s="151"/>
+      <c r="F41" s="151"/>
+      <c r="G41" s="151"/>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="151" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>